<commit_message>
Fix plru to work
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
   <si>
     <t>Cache size</t>
   </si>
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -100,6 +100,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,23 +410,23 @@
         <v>FIB RANDOM</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="H2" s="5" t="str">
         <f>CONCATENATE(A1, " PLRU")</f>
         <v>FIB PLRU</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -526,12 +529,13 @@
         <v>300</v>
       </c>
       <c r="K5">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="L5">
         <v>300</v>
       </c>
       <c r="M5">
+        <f>J5</f>
         <v>300</v>
       </c>
     </row>
@@ -561,13 +565,13 @@
         <v>198</v>
       </c>
       <c r="K6">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="L6">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="M6">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -596,13 +600,13 @@
         <v>172</v>
       </c>
       <c r="K7">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="L7">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="M7">
-        <v>300</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -634,10 +638,10 @@
         <v>172</v>
       </c>
       <c r="L8">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="M8">
-        <v>300</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -671,8 +675,8 @@
       <c r="L9">
         <v>172</v>
       </c>
-      <c r="M9">
-        <v>300</v>
+      <c r="M9" s="3">
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -701,14 +705,14 @@
         <f t="shared" si="0"/>
         <v>172</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>172</v>
       </c>
       <c r="L10" s="3">
         <v>172</v>
       </c>
       <c r="M10" s="3">
-        <v>300</v>
+        <v>172</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -764,23 +768,23 @@
         <v>SUM RANDOM</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="H14" s="5" t="str">
         <f>CONCATENATE(A13, " PLRU")</f>
         <v>SUM PLRU</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -936,7 +940,7 @@
         <v>307</v>
       </c>
       <c r="M18">
-        <v>307</v>
+        <v>215</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -971,10 +975,10 @@
         <v>212</v>
       </c>
       <c r="L19">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="M19">
-        <v>307</v>
+        <v>212</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1012,7 +1016,7 @@
         <v>212</v>
       </c>
       <c r="M20">
-        <v>307</v>
+        <v>212</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1050,7 +1054,7 @@
         <v>212</v>
       </c>
       <c r="M21">
-        <v>307</v>
+        <v>212</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1082,14 +1086,14 @@
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="K22" s="3">
-        <v>212</v>
-      </c>
-      <c r="L22" s="3">
-        <v>212</v>
-      </c>
-      <c r="M22" s="3">
-        <v>307</v>
+      <c r="K22">
+        <v>212</v>
+      </c>
+      <c r="L22">
+        <v>212</v>
+      </c>
+      <c r="M22">
+        <v>212</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -1145,23 +1149,23 @@
         <v>PRIMES RANDOM</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="H26" s="5" t="str">
         <f>CONCATENATE(A25, " PLRU")</f>
         <v>PRIMES PLRU</v>
       </c>
       <c r="I26" s="5"/>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -1273,7 +1277,7 @@
         <v>1629</v>
       </c>
       <c r="K29">
-        <v>1632</v>
+        <v>1584</v>
       </c>
       <c r="L29">
         <v>1632</v>
@@ -1311,13 +1315,13 @@
         <v>1125</v>
       </c>
       <c r="K30">
-        <v>1629</v>
+        <v>1510</v>
       </c>
       <c r="L30">
-        <v>1632</v>
+        <v>1579</v>
       </c>
       <c r="M30">
-        <v>1632</v>
+        <v>1170</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -1349,13 +1353,13 @@
         <v>866</v>
       </c>
       <c r="K31">
-        <v>1251</v>
+        <v>1057</v>
       </c>
       <c r="L31">
-        <v>1629</v>
+        <v>1254</v>
       </c>
       <c r="M31">
-        <v>1632</v>
+        <v>898</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
@@ -1387,13 +1391,13 @@
         <v>860</v>
       </c>
       <c r="K32">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="L32">
-        <v>1251</v>
+        <v>1024</v>
       </c>
       <c r="M32">
-        <v>1632</v>
+        <v>860</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -1428,10 +1432,10 @@
         <v>860</v>
       </c>
       <c r="L33">
-        <v>866</v>
+        <v>890</v>
       </c>
       <c r="M33">
-        <v>1632</v>
+        <v>860</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
@@ -1470,7 +1474,7 @@
         <v>860</v>
       </c>
       <c r="M34">
-        <v>1632</v>
+        <v>860</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
@@ -1482,26 +1486,347 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
     </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="str">
+        <f>CONCATENATE(A37, " RANDOM")</f>
+        <v>PRIMES RANDOM</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="H38" s="5" t="str">
+        <f>CONCATENATE(A37, " PLRU")</f>
+        <v>PRIMES PLRU</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>5</v>
+      </c>
+      <c r="M39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1632</v>
+      </c>
+      <c r="D40">
+        <f>C40</f>
+        <v>1632</v>
+      </c>
+      <c r="E40">
+        <f>C40</f>
+        <v>1632</v>
+      </c>
+      <c r="F40">
+        <f>C40</f>
+        <v>1632</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f>C40</f>
+        <v>1632</v>
+      </c>
+      <c r="K40">
+        <f>J40</f>
+        <v>1632</v>
+      </c>
+      <c r="L40">
+        <f>J40</f>
+        <v>1632</v>
+      </c>
+      <c r="M40">
+        <f>J40</f>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="4">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>1629</v>
+      </c>
+      <c r="D41">
+        <v>1633</v>
+      </c>
+      <c r="E41">
+        <v>1632</v>
+      </c>
+      <c r="F41">
+        <v>1632</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="4">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <f t="shared" ref="J41:J46" si="3">C41</f>
+        <v>1629</v>
+      </c>
+      <c r="K41">
+        <v>1584</v>
+      </c>
+      <c r="L41">
+        <v>1632</v>
+      </c>
+      <c r="M41">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="4">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>1125</v>
+      </c>
+      <c r="D42">
+        <v>1335</v>
+      </c>
+      <c r="E42">
+        <v>1475</v>
+      </c>
+      <c r="F42">
+        <v>1373</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" s="4">
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="3"/>
+        <v>1125</v>
+      </c>
+      <c r="K42">
+        <v>1510</v>
+      </c>
+      <c r="L42">
+        <v>1579</v>
+      </c>
+      <c r="M42">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="4">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>866</v>
+      </c>
+      <c r="D43">
+        <v>1331</v>
+      </c>
+      <c r="E43">
+        <v>1371</v>
+      </c>
+      <c r="F43">
+        <v>897</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="4">
+        <v>16</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="3"/>
+        <v>866</v>
+      </c>
+      <c r="K43">
+        <v>1057</v>
+      </c>
+      <c r="L43">
+        <v>1254</v>
+      </c>
+      <c r="M43">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="4">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>860</v>
+      </c>
+      <c r="D44">
+        <v>1008</v>
+      </c>
+      <c r="E44">
+        <v>985</v>
+      </c>
+      <c r="F44">
+        <v>860</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="4">
+        <v>32</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="3"/>
+        <v>860</v>
+      </c>
+      <c r="K44">
+        <v>873</v>
+      </c>
+      <c r="L44">
+        <v>1024</v>
+      </c>
+      <c r="M44">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="4">
+        <v>64</v>
+      </c>
+      <c r="C45">
+        <v>860</v>
+      </c>
+      <c r="D45">
+        <v>923</v>
+      </c>
+      <c r="E45">
+        <v>883</v>
+      </c>
+      <c r="F45">
+        <v>860</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" s="4">
+        <v>64</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="3"/>
+        <v>860</v>
+      </c>
+      <c r="K45">
+        <v>860</v>
+      </c>
+      <c r="L45">
+        <v>890</v>
+      </c>
+      <c r="M45">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="4">
+        <v>128</v>
+      </c>
+      <c r="C46" s="3">
+        <v>860</v>
+      </c>
+      <c r="D46" s="3">
+        <v>923</v>
+      </c>
+      <c r="E46" s="3">
+        <v>877</v>
+      </c>
+      <c r="F46" s="3">
+        <v>860</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="4">
+        <v>128</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="3"/>
+        <v>860</v>
+      </c>
+      <c r="K46" s="3">
+        <v>860</v>
+      </c>
+      <c r="L46" s="3">
+        <v>860</v>
+      </c>
+      <c r="M46">
+        <v>860</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="24">
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="H40:H46"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="H16:H22"/>
     <mergeCell ref="A26:B27"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="H26:I27"/>
     <mergeCell ref="J26:M26"/>
     <mergeCell ref="A28:A34"/>
     <mergeCell ref="H28:H34"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="A4:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
done this shit note LW still not working after SW hahahahaha :D
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Cache size</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>PRIMES</t>
+  </si>
+  <si>
+    <t>BITWISE</t>
+  </si>
+  <si>
+    <t>GCD</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -97,6 +103,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,32 +417,32 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="7" t="str">
         <f>CONCATENATE(A1, " RANDOM")</f>
         <v>FIB RANDOM</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="H2" s="5" t="str">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="7" t="str">
         <f>CONCATENATE(A1, " PLRU")</f>
         <v>FIB PLRU</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -443,8 +455,8 @@
       <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" t="s">
         <v>3</v>
       </c>
@@ -459,7 +471,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -480,7 +492,7 @@
         <f>C4</f>
         <v>300</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="1">
@@ -504,7 +516,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -520,7 +532,7 @@
       <c r="F5">
         <v>300</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="1">
         <v>4</v>
       </c>
@@ -540,7 +552,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1">
         <v>8</v>
       </c>
@@ -556,7 +568,7 @@
       <c r="F6">
         <v>300</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="1">
         <v>8</v>
       </c>
@@ -575,7 +587,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1">
         <v>16</v>
       </c>
@@ -591,7 +603,7 @@
       <c r="F7">
         <v>172</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="1">
         <v>16</v>
       </c>
@@ -610,7 +622,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1">
         <v>32</v>
       </c>
@@ -626,7 +638,7 @@
       <c r="F8">
         <v>172</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="1">
         <v>32</v>
       </c>
@@ -645,7 +657,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1">
         <v>64</v>
       </c>
@@ -661,7 +673,7 @@
       <c r="F9">
         <v>172</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="1">
         <v>64</v>
       </c>
@@ -680,7 +692,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1">
         <v>128</v>
       </c>
@@ -697,7 +709,7 @@
         <v>172</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="2">
         <v>128</v>
       </c>
@@ -763,35 +775,35 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="str">
+      <c r="A14" s="7" t="str">
         <f>CONCATENATE(A13, " RANDOM")</f>
         <v>SUM RANDOM</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="H14" s="5" t="str">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="7" t="str">
         <f>CONCATENATE(A13, " PLRU")</f>
         <v>SUM PLRU</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6" t="s">
+      <c r="I14" s="7"/>
+      <c r="J14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -804,8 +816,8 @@
       <c r="F15" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
       <c r="J15" t="s">
         <v>3</v>
       </c>
@@ -823,7 +835,7 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="2">
@@ -844,7 +856,7 @@
         <f>C16</f>
         <v>307</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="2">
@@ -871,7 +883,7 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2">
         <v>4</v>
       </c>
@@ -887,7 +899,7 @@
       <c r="F17">
         <v>307</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="2">
         <v>4</v>
       </c>
@@ -909,7 +921,7 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2">
         <v>8</v>
       </c>
@@ -925,7 +937,7 @@
       <c r="F18">
         <v>212</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="2">
         <v>8</v>
       </c>
@@ -947,7 +959,7 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -963,7 +975,7 @@
       <c r="F19">
         <v>212</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="2">
         <v>16</v>
       </c>
@@ -985,7 +997,7 @@
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2">
         <v>32</v>
       </c>
@@ -1001,7 +1013,7 @@
       <c r="F20">
         <v>212</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="2">
         <v>32</v>
       </c>
@@ -1023,7 +1035,7 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2">
         <v>64</v>
       </c>
@@ -1039,7 +1051,7 @@
       <c r="F21">
         <v>212</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="2">
         <v>64</v>
       </c>
@@ -1061,7 +1073,7 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2">
         <v>128</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>212</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="2">
         <v>128</v>
       </c>
@@ -1144,35 +1156,35 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="str">
+      <c r="A26" s="7" t="str">
         <f>CONCATENATE(A25, " RANDOM")</f>
         <v>PRIMES RANDOM</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="H26" s="5" t="str">
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="H26" s="7" t="str">
         <f>CONCATENATE(A25, " PLRU")</f>
         <v>PRIMES PLRU</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6" t="s">
+      <c r="I26" s="7"/>
+      <c r="J26" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
       <c r="C27" t="s">
         <v>3</v>
       </c>
@@ -1185,8 +1197,8 @@
       <c r="F27" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
       <c r="J27" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1216,7 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="2">
@@ -1225,7 +1237,7 @@
         <f>C28</f>
         <v>1632</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="2">
@@ -1252,7 +1264,7 @@
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="2">
         <v>4</v>
       </c>
@@ -1268,7 +1280,7 @@
       <c r="F29">
         <v>1632</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="2">
         <v>4</v>
       </c>
@@ -1290,7 +1302,7 @@
       <c r="P29" s="3"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="2">
         <v>8</v>
       </c>
@@ -1306,7 +1318,7 @@
       <c r="F30">
         <v>1373</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="2">
         <v>8</v>
       </c>
@@ -1328,7 +1340,7 @@
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="2">
         <v>16</v>
       </c>
@@ -1344,7 +1356,7 @@
       <c r="F31">
         <v>897</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="7"/>
       <c r="I31" s="2">
         <v>16</v>
       </c>
@@ -1366,7 +1378,7 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="2">
         <v>32</v>
       </c>
@@ -1382,7 +1394,7 @@
       <c r="F32">
         <v>860</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="2">
         <v>32</v>
       </c>
@@ -1404,7 +1416,7 @@
       <c r="P32" s="3"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="2">
         <v>64</v>
       </c>
@@ -1420,7 +1432,7 @@
       <c r="F33">
         <v>860</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="2">
         <v>64</v>
       </c>
@@ -1442,7 +1454,7 @@
       <c r="P33" s="3"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2">
         <v>128</v>
       </c>
@@ -1459,7 +1471,7 @@
         <v>860</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="5"/>
+      <c r="H34" s="7"/>
       <c r="I34" s="2">
         <v>128</v>
       </c>
@@ -1488,36 +1500,36 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="str">
+      <c r="A38" s="7" t="str">
         <f>CONCATENATE(A37, " RANDOM")</f>
-        <v>PRIMES RANDOM</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="6" t="s">
+        <v>BITWISE RANDOM</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="H38" s="5" t="str">
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="H38" s="7" t="str">
         <f>CONCATENATE(A37, " PLRU")</f>
-        <v>PRIMES PLRU</v>
-      </c>
-      <c r="I38" s="5"/>
-      <c r="J38" s="6" t="s">
+        <v>BITWISE PLRU</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
       <c r="C39" t="s">
         <v>3</v>
       </c>
@@ -1530,8 +1542,8 @@
       <c r="F39" t="s">
         <v>2</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
       <c r="J39" t="s">
         <v>3</v>
       </c>
@@ -1546,28 +1558,28 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="4">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="D40">
         <f>C40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="E40">
         <f>C40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="F40">
         <f>C40</f>
-        <v>1632</v>
-      </c>
-      <c r="H40" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="4">
@@ -1575,234 +1587,579 @@
       </c>
       <c r="J40">
         <f>C40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="K40">
         <f>J40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="L40">
         <f>J40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="M40">
         <f>J40</f>
-        <v>1632</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="4">
         <v>4</v>
       </c>
       <c r="C41">
-        <v>1629</v>
+        <v>105</v>
       </c>
       <c r="D41">
-        <v>1633</v>
+        <v>105</v>
       </c>
       <c r="E41">
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="F41">
-        <v>1632</v>
-      </c>
-      <c r="H41" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="H41" s="7"/>
       <c r="I41" s="4">
         <v>4</v>
       </c>
       <c r="J41">
         <f t="shared" ref="J41:J46" si="3">C41</f>
-        <v>1629</v>
+        <v>105</v>
       </c>
       <c r="K41">
-        <v>1584</v>
+        <v>105</v>
       </c>
       <c r="L41">
-        <v>1632</v>
+        <v>105</v>
       </c>
       <c r="M41">
-        <v>1632</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="4">
         <v>8</v>
       </c>
       <c r="C42">
-        <v>1125</v>
+        <v>105</v>
       </c>
       <c r="D42">
-        <v>1335</v>
+        <v>105</v>
       </c>
       <c r="E42">
-        <v>1475</v>
+        <v>105</v>
       </c>
       <c r="F42">
-        <v>1373</v>
-      </c>
-      <c r="H42" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="H42" s="7"/>
       <c r="I42" s="4">
         <v>8</v>
       </c>
       <c r="J42">
         <f t="shared" si="3"/>
-        <v>1125</v>
+        <v>105</v>
       </c>
       <c r="K42">
-        <v>1510</v>
+        <v>105</v>
       </c>
       <c r="L42">
-        <v>1579</v>
+        <v>105</v>
       </c>
       <c r="M42">
-        <v>1170</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="4">
         <v>16</v>
       </c>
       <c r="C43">
-        <v>866</v>
+        <v>105</v>
       </c>
       <c r="D43">
-        <v>1331</v>
+        <v>105</v>
       </c>
       <c r="E43">
-        <v>1371</v>
+        <v>105</v>
       </c>
       <c r="F43">
-        <v>897</v>
-      </c>
-      <c r="H43" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="H43" s="7"/>
       <c r="I43" s="4">
         <v>16</v>
       </c>
       <c r="J43">
         <f t="shared" si="3"/>
-        <v>866</v>
+        <v>105</v>
       </c>
       <c r="K43">
-        <v>1057</v>
+        <v>105</v>
       </c>
       <c r="L43">
-        <v>1254</v>
+        <v>105</v>
       </c>
       <c r="M43">
-        <v>898</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="4">
         <v>32</v>
       </c>
       <c r="C44">
-        <v>860</v>
+        <v>105</v>
       </c>
       <c r="D44">
-        <v>1008</v>
+        <v>105</v>
       </c>
       <c r="E44">
-        <v>985</v>
+        <v>105</v>
       </c>
       <c r="F44">
-        <v>860</v>
-      </c>
-      <c r="H44" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="H44" s="7"/>
       <c r="I44" s="4">
         <v>32</v>
       </c>
       <c r="J44">
         <f t="shared" si="3"/>
-        <v>860</v>
+        <v>105</v>
       </c>
       <c r="K44">
-        <v>873</v>
+        <v>105</v>
       </c>
       <c r="L44">
-        <v>1024</v>
+        <v>105</v>
       </c>
       <c r="M44">
-        <v>860</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="4">
         <v>64</v>
       </c>
       <c r="C45">
-        <v>860</v>
+        <v>105</v>
       </c>
       <c r="D45">
-        <v>923</v>
+        <v>105</v>
       </c>
       <c r="E45">
-        <v>883</v>
+        <v>105</v>
       </c>
       <c r="F45">
-        <v>860</v>
-      </c>
-      <c r="H45" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="H45" s="7"/>
       <c r="I45" s="4">
         <v>64</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
-        <v>860</v>
+        <v>105</v>
       </c>
       <c r="K45">
-        <v>860</v>
+        <v>105</v>
       </c>
       <c r="L45">
-        <v>890</v>
+        <v>105</v>
       </c>
       <c r="M45">
-        <v>860</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="4">
         <v>128</v>
       </c>
-      <c r="C46" s="3">
-        <v>860</v>
-      </c>
-      <c r="D46" s="3">
-        <v>923</v>
-      </c>
-      <c r="E46" s="3">
-        <v>877</v>
-      </c>
-      <c r="F46" s="3">
-        <v>860</v>
+      <c r="C46">
+        <v>105</v>
+      </c>
+      <c r="D46">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>105</v>
+      </c>
+      <c r="F46">
+        <v>105</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="5"/>
+      <c r="H46" s="7"/>
       <c r="I46" s="4">
         <v>128</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="3"/>
-        <v>860</v>
-      </c>
-      <c r="K46" s="3">
-        <v>860</v>
-      </c>
-      <c r="L46" s="3">
-        <v>860</v>
+        <f>F46</f>
+        <v>105</v>
+      </c>
+      <c r="K46">
+        <v>105</v>
+      </c>
+      <c r="L46">
+        <v>105</v>
       </c>
       <c r="M46">
-        <v>860</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="str">
+        <f>CONCATENATE(A49, " RANDOM")</f>
+        <v>GCD RANDOM</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="H50" s="7" t="str">
+        <f>CONCATENATE(A49, " PLRU")</f>
+        <v>GCD PLRU</v>
+      </c>
+      <c r="I50" s="7"/>
+      <c r="J50" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" t="s">
+        <v>3</v>
+      </c>
+      <c r="K51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L51" t="s">
+        <v>5</v>
+      </c>
+      <c r="M51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>165</v>
+      </c>
+      <c r="D52">
+        <f>C52</f>
+        <v>165</v>
+      </c>
+      <c r="E52">
+        <f>C52</f>
+        <v>165</v>
+      </c>
+      <c r="F52">
+        <f>C52</f>
+        <v>165</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="5">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f>C52</f>
+        <v>165</v>
+      </c>
+      <c r="K52">
+        <f>J52</f>
+        <v>165</v>
+      </c>
+      <c r="L52">
+        <f>J52</f>
+        <v>165</v>
+      </c>
+      <c r="M52">
+        <f>J52</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="5">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>152</v>
+      </c>
+      <c r="D53">
+        <v>165</v>
+      </c>
+      <c r="E53">
+        <v>165</v>
+      </c>
+      <c r="F53">
+        <v>165</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="5">
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <v>152</v>
+      </c>
+      <c r="K53">
+        <v>165</v>
+      </c>
+      <c r="L53">
+        <v>165</v>
+      </c>
+      <c r="M53">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="5">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>128</v>
+      </c>
+      <c r="D54">
+        <v>165</v>
+      </c>
+      <c r="E54">
+        <v>165</v>
+      </c>
+      <c r="F54">
+        <v>128</v>
+      </c>
+      <c r="H54" s="7"/>
+      <c r="I54" s="5">
+        <v>8</v>
+      </c>
+      <c r="J54">
+        <v>128</v>
+      </c>
+      <c r="K54">
+        <v>146</v>
+      </c>
+      <c r="L54">
+        <v>165</v>
+      </c>
+      <c r="M54">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="5">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <v>128</v>
+      </c>
+      <c r="D55">
+        <v>165</v>
+      </c>
+      <c r="E55">
+        <v>153</v>
+      </c>
+      <c r="F55">
+        <v>128</v>
+      </c>
+      <c r="H55" s="7"/>
+      <c r="I55" s="5">
+        <v>16</v>
+      </c>
+      <c r="J55">
+        <v>128</v>
+      </c>
+      <c r="K55">
+        <v>128</v>
+      </c>
+      <c r="L55">
+        <v>131</v>
+      </c>
+      <c r="M55">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="5">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>128</v>
+      </c>
+      <c r="D56">
+        <v>165</v>
+      </c>
+      <c r="E56">
+        <v>140</v>
+      </c>
+      <c r="F56">
+        <v>128</v>
+      </c>
+      <c r="H56" s="7"/>
+      <c r="I56" s="5">
+        <v>32</v>
+      </c>
+      <c r="J56">
+        <v>128</v>
+      </c>
+      <c r="K56">
+        <v>128</v>
+      </c>
+      <c r="L56">
+        <v>128</v>
+      </c>
+      <c r="M56">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="5">
+        <v>64</v>
+      </c>
+      <c r="C57">
+        <v>128</v>
+      </c>
+      <c r="D57">
+        <v>165</v>
+      </c>
+      <c r="E57">
+        <v>148</v>
+      </c>
+      <c r="F57">
+        <v>128</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="5">
+        <v>64</v>
+      </c>
+      <c r="J57">
+        <v>128</v>
+      </c>
+      <c r="K57">
+        <v>128</v>
+      </c>
+      <c r="L57">
+        <v>128</v>
+      </c>
+      <c r="M57">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="5">
+        <v>128</v>
+      </c>
+      <c r="C58">
+        <v>128</v>
+      </c>
+      <c r="D58">
+        <v>165</v>
+      </c>
+      <c r="E58">
+        <v>148</v>
+      </c>
+      <c r="F58">
+        <v>128</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="5">
+        <v>128</v>
+      </c>
+      <c r="J58" s="3">
+        <v>128</v>
+      </c>
+      <c r="K58" s="3">
+        <v>128</v>
+      </c>
+      <c r="L58">
+        <v>128</v>
+      </c>
+      <c r="M58">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H50:I51"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="H52:H58"/>
     <mergeCell ref="A38:B39"/>
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="H38:I39"/>

</xml_diff>

<commit_message>
Fix two way and four way associativity
</commit_message>
<xml_diff>
--- a/Evaluations.xlsx
+++ b/Evaluations.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+      <selection activeCell="J50" sqref="J50:M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>300</v>
       </c>
       <c r="K5">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="L5">
         <v>300</v>
@@ -560,10 +560,10 @@
         <v>198</v>
       </c>
       <c r="D6">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E6">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F6">
         <v>300</v>
@@ -577,10 +577,10 @@
         <v>198</v>
       </c>
       <c r="K6">
-        <v>285</v>
+        <v>216</v>
       </c>
       <c r="L6">
-        <v>285</v>
+        <v>221</v>
       </c>
       <c r="M6">
         <v>229</v>
@@ -595,10 +595,10 @@
         <v>172</v>
       </c>
       <c r="D7">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="E7">
-        <v>272</v>
+        <v>193</v>
       </c>
       <c r="F7">
         <v>172</v>
@@ -612,10 +612,10 @@
         <v>172</v>
       </c>
       <c r="K7">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="L7">
-        <v>243</v>
+        <v>172</v>
       </c>
       <c r="M7">
         <v>172</v>
@@ -630,10 +630,10 @@
         <v>172</v>
       </c>
       <c r="D8">
-        <v>267</v>
+        <v>172</v>
       </c>
       <c r="E8">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="F8">
         <v>172</v>
@@ -650,7 +650,7 @@
         <v>172</v>
       </c>
       <c r="L8">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="M8">
         <v>172</v>
@@ -665,10 +665,10 @@
         <v>172</v>
       </c>
       <c r="D9">
-        <v>267</v>
+        <v>172</v>
       </c>
       <c r="E9">
-        <v>282</v>
+        <v>172</v>
       </c>
       <c r="F9">
         <v>172</v>
@@ -699,11 +699,11 @@
       <c r="C10" s="3">
         <v>172</v>
       </c>
-      <c r="D10" s="3">
-        <v>267</v>
+      <c r="D10">
+        <v>172</v>
       </c>
       <c r="E10" s="3">
-        <v>282</v>
+        <v>172</v>
       </c>
       <c r="F10">
         <v>172</v>
@@ -946,10 +946,10 @@
         <v>212</v>
       </c>
       <c r="K18">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="L18">
-        <v>307</v>
+        <v>215</v>
       </c>
       <c r="M18">
         <v>215</v>
@@ -970,7 +970,7 @@
         <v>212</v>
       </c>
       <c r="E19">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="F19">
         <v>212</v>
@@ -987,7 +987,7 @@
         <v>212</v>
       </c>
       <c r="L19">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="M19">
         <v>212</v>
@@ -1005,10 +1005,10 @@
         <v>212</v>
       </c>
       <c r="D20">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E20">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F20">
         <v>212</v>
@@ -1043,10 +1043,10 @@
         <v>212</v>
       </c>
       <c r="D21">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E21">
-        <v>258</v>
+        <v>212</v>
       </c>
       <c r="F21">
         <v>212</v>
@@ -1081,10 +1081,10 @@
         <v>212</v>
       </c>
       <c r="D22">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E22">
-        <v>258</v>
+        <v>212</v>
       </c>
       <c r="F22">
         <v>212</v>
@@ -1289,7 +1289,7 @@
         <v>1629</v>
       </c>
       <c r="K29">
-        <v>1584</v>
+        <v>1632</v>
       </c>
       <c r="L29">
         <v>1632</v>
@@ -1310,10 +1310,10 @@
         <v>1125</v>
       </c>
       <c r="D30">
-        <v>1335</v>
+        <v>1259</v>
       </c>
       <c r="E30">
-        <v>1475</v>
+        <v>1204</v>
       </c>
       <c r="F30">
         <v>1373</v>
@@ -1327,10 +1327,10 @@
         <v>1125</v>
       </c>
       <c r="K30">
-        <v>1510</v>
+        <v>1152</v>
       </c>
       <c r="L30">
-        <v>1579</v>
+        <v>1204</v>
       </c>
       <c r="M30">
         <v>1170</v>
@@ -1348,10 +1348,10 @@
         <v>866</v>
       </c>
       <c r="D31">
-        <v>1331</v>
+        <v>874</v>
       </c>
       <c r="E31">
-        <v>1371</v>
+        <v>884</v>
       </c>
       <c r="F31">
         <v>897</v>
@@ -1365,10 +1365,10 @@
         <v>866</v>
       </c>
       <c r="K31">
-        <v>1057</v>
+        <v>877</v>
       </c>
       <c r="L31">
-        <v>1254</v>
+        <v>884</v>
       </c>
       <c r="M31">
         <v>898</v>
@@ -1386,10 +1386,10 @@
         <v>860</v>
       </c>
       <c r="D32">
-        <v>1008</v>
+        <v>863</v>
       </c>
       <c r="E32">
-        <v>985</v>
+        <v>860</v>
       </c>
       <c r="F32">
         <v>860</v>
@@ -1403,10 +1403,10 @@
         <v>860</v>
       </c>
       <c r="K32">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="L32">
-        <v>1024</v>
+        <v>860</v>
       </c>
       <c r="M32">
         <v>860</v>
@@ -1424,10 +1424,10 @@
         <v>860</v>
       </c>
       <c r="D33">
-        <v>923</v>
+        <v>860</v>
       </c>
       <c r="E33">
-        <v>883</v>
+        <v>860</v>
       </c>
       <c r="F33">
         <v>860</v>
@@ -1444,7 +1444,7 @@
         <v>860</v>
       </c>
       <c r="L33">
-        <v>890</v>
+        <v>860</v>
       </c>
       <c r="M33">
         <v>860</v>
@@ -1462,10 +1462,10 @@
         <v>860</v>
       </c>
       <c r="D34" s="3">
-        <v>923</v>
+        <v>860</v>
       </c>
       <c r="E34" s="3">
-        <v>877</v>
+        <v>860</v>
       </c>
       <c r="F34" s="3">
         <v>860</v>
@@ -1494,6 +1494,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
@@ -1624,7 +1625,7 @@
         <v>4</v>
       </c>
       <c r="J41">
-        <f t="shared" ref="J41:J46" si="3">C41</f>
+        <f t="shared" ref="J41:J45" si="3">C41</f>
         <v>105</v>
       </c>
       <c r="K41">
@@ -1910,19 +1911,19 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D52">
         <f>C52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="E52">
         <f>C52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="F52">
         <f>C52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>0</v>
@@ -1932,19 +1933,19 @@
       </c>
       <c r="J52">
         <f>C52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="K52">
         <f>J52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="L52">
         <f>J52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="M52">
         <f>J52</f>
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -1953,32 +1954,33 @@
         <v>4</v>
       </c>
       <c r="C53">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D53">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="E53">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="F53">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="5">
         <v>4</v>
       </c>
       <c r="J53">
-        <v>152</v>
+        <f>C53</f>
+        <v>138</v>
       </c>
       <c r="K53">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="L53">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="M53">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -1987,32 +1989,33 @@
         <v>8</v>
       </c>
       <c r="C54">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D54">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E54">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="F54">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="5">
         <v>8</v>
       </c>
       <c r="J54">
-        <v>128</v>
+        <f t="shared" ref="J54:J58" si="4">C54</f>
+        <v>123</v>
       </c>
       <c r="K54">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="L54">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="M54">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -2021,32 +2024,33 @@
         <v>16</v>
       </c>
       <c r="C55">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D55">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="E55">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="F55">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="5">
         <v>16</v>
       </c>
       <c r="J55">
-        <v>128</v>
+        <f t="shared" si="4"/>
+        <v>123</v>
       </c>
       <c r="K55">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L55">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="M55">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -2055,32 +2059,33 @@
         <v>32</v>
       </c>
       <c r="C56">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D56">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="E56">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="F56">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="5">
         <v>32</v>
       </c>
       <c r="J56">
-        <v>128</v>
+        <f t="shared" si="4"/>
+        <v>123</v>
       </c>
       <c r="K56">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L56">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="M56">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -2089,32 +2094,33 @@
         <v>64</v>
       </c>
       <c r="C57">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D57">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="E57">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F57">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="5">
         <v>64</v>
       </c>
       <c r="J57">
-        <v>128</v>
+        <f t="shared" si="4"/>
+        <v>123</v>
       </c>
       <c r="K57">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L57">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="M57">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -2123,67 +2129,68 @@
         <v>128</v>
       </c>
       <c r="C58">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D58">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="E58">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F58">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="7"/>
       <c r="I58" s="5">
         <v>128</v>
       </c>
-      <c r="J58" s="3">
-        <v>128</v>
-      </c>
-      <c r="K58" s="3">
-        <v>128</v>
+      <c r="J58">
+        <f t="shared" si="4"/>
+        <v>123</v>
+      </c>
+      <c r="K58">
+        <v>123</v>
       </c>
       <c r="L58">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="M58">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="H26:I27"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="H28:H34"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="H40:H46"/>
     <mergeCell ref="A50:B51"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="H50:I51"/>
     <mergeCell ref="J50:M50"/>
     <mergeCell ref="A52:A58"/>
     <mergeCell ref="H52:H58"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="H38:I39"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="H40:H46"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="H26:I27"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="H28:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>